<commit_message>
clean up and add src
</commit_message>
<xml_diff>
--- a/HiWi_Orga/Stundennachweise/Stundenübersicht.xlsx
+++ b/HiWi_Orga/Stundennachweise/Stundenübersicht.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Envimaster\DWA\HiWi_Orga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Envimaster\DWA\HiWi_Orga\Stundennachweise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FCC6BF-BBF8-4BF2-92AF-6719AEDD6E10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A671E76-3579-411B-9B85-4443D9309332}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8955" xr2:uid="{85153F1B-7004-4098-957F-C1553457F176}"/>
   </bookViews>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED71B0D8-667D-4529-A9C1-4C12D1464679}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,6 +770,9 @@
       <c r="A14" t="s">
         <v>10</v>
       </c>
+      <c r="B14" s="2">
+        <v>27.67</v>
+      </c>
       <c r="E14" t="s">
         <v>23</v>
       </c>
@@ -798,7 +801,7 @@
       </c>
       <c r="B19" s="5">
         <f>B4-SUM(B5:B14)</f>
-        <v>112.85000000000002</v>
+        <v>85.18</v>
       </c>
       <c r="C19" s="5">
         <f>C4-SUM(C5:C14)</f>

</xml_diff>

<commit_message>
update Stundenzettel and src
</commit_message>
<xml_diff>
--- a/HiWi_Orga/Stundennachweise/Stundenübersicht.xlsx
+++ b/HiWi_Orga/Stundennachweise/Stundenübersicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Envimaster\DWA\HiWi_Orga\Stundennachweise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A671E76-3579-411B-9B85-4443D9309332}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EA3D76-3FCC-4331-8A8E-369DBB079824}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8955" xr2:uid="{85153F1B-7004-4098-957F-C1553457F176}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>HiWi Stundenübersicht</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Al</t>
+  </si>
+  <si>
+    <t>JR</t>
+  </si>
+  <si>
+    <t>Soll bis 31.3.23</t>
   </si>
 </sst>
 </file>
@@ -185,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -193,8 +199,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +516,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,6 +543,9 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
       <c r="G2" t="s">
@@ -549,6 +556,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
       <c r="G3" s="4"/>
       <c r="H3" t="s">
         <v>22</v>
@@ -571,6 +581,10 @@
         <v>400</v>
       </c>
       <c r="E4" s="5">
+        <f>(43/2)+3*43</f>
+        <v>150.5</v>
+      </c>
+      <c r="F4" s="5">
         <v>225</v>
       </c>
       <c r="G4" s="1"/>
@@ -591,7 +605,10 @@
       <c r="D5" s="2">
         <v>15.5</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2">
         <v>28</v>
       </c>
       <c r="G5" s="3"/>
@@ -612,7 +629,10 @@
       <c r="D6" s="2">
         <v>33</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2">
         <v>29.43</v>
       </c>
       <c r="G6" s="2"/>
@@ -633,7 +653,10 @@
       <c r="D7" s="2">
         <v>30</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2">
         <v>30.8</v>
       </c>
     </row>
@@ -650,10 +673,12 @@
       <c r="D8" s="2">
         <v>26.5</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2">
         <v>30.4</v>
       </c>
-      <c r="F8" s="7"/>
       <c r="G8" t="s">
         <v>24</v>
       </c>
@@ -671,10 +696,12 @@
       <c r="D9" s="2">
         <v>28</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="2">
         <v>40.07</v>
       </c>
-      <c r="F9" s="7"/>
       <c r="G9" t="s">
         <v>13</v>
       </c>
@@ -695,10 +722,12 @@
       <c r="D10" s="2">
         <v>37.5</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2">
         <v>30.95</v>
       </c>
-      <c r="F10" s="7"/>
       <c r="G10" t="s">
         <v>28</v>
       </c>
@@ -719,10 +748,12 @@
       <c r="D11" s="2">
         <v>24.25</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="2">
         <v>19.649999999999999</v>
       </c>
-      <c r="F11" s="7"/>
       <c r="G11" t="s">
         <v>12</v>
       </c>
@@ -743,10 +774,12 @@
       <c r="D12" s="2">
         <v>35.25</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2">
         <v>15.53</v>
       </c>
-      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -764,7 +797,9 @@
       <c r="E13" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -776,26 +811,26 @@
       <c r="E14" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
@@ -811,8 +846,12 @@
         <f>D4-SUM(D5:D14)</f>
         <v>132.75</v>
       </c>
-      <c r="E19" s="6">
-        <f>E4-SUM(E5:E14)</f>
+      <c r="E19">
+        <f>E4-E15-E16-E17</f>
+        <v>150.5</v>
+      </c>
+      <c r="F19" s="6">
+        <f>F4-SUM(F5:F14)</f>
         <v>0.17000000000001592</v>
       </c>
     </row>

</xml_diff>